<commit_message>
Updated sample 75 water bridges results
</commit_message>
<xml_diff>
--- a/double_water_bridges_75.xlsx
+++ b/double_water_bridges_75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihan\Documents\Uni\Fall 2022\CHE 293\Project\Water bridges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D680249B-5398-435D-B768-B4AB32F2BC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9A85E8-7A0F-42D8-AB00-C9825851485A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="124">
   <si>
     <t>75-r4-50k-140k-merged-22</t>
   </si>
@@ -404,43 +404,7 @@
     <t>Bridging</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
     <t>Files</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>A0025B0035</t>
-  </si>
-  <si>
-    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -971,14 +935,74 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="22">
     <dxf>
       <font>
-        <color theme="7" tint="-0.499984740745262"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE8DFA0"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF33CC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -994,71 +1018,31 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE8DFA0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4D4D4D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF33CC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1159,106 +1143,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFE8DFA0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF33CC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1591,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O239"/>
+  <dimension ref="A1:N239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1489,7 @@
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1615,11 +1499,8 @@
       <c r="N1" t="s">
         <v>123</v>
       </c>
-      <c r="O1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1638,14 +1519,11 @@
       <c r="M2" t="s">
         <v>61</v>
       </c>
-      <c r="N2" t="s">
-        <v>135</v>
-      </c>
-      <c r="O2">
+      <c r="N2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1675,14 +1553,11 @@
       <c r="M3" t="s">
         <v>59</v>
       </c>
-      <c r="N3" t="s">
-        <v>125</v>
-      </c>
-      <c r="O3">
+      <c r="N3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1711,14 +1586,11 @@
       <c r="M4" t="s">
         <v>62</v>
       </c>
-      <c r="N4" t="s">
-        <v>126</v>
-      </c>
-      <c r="O4">
+      <c r="N4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1748,14 +1620,11 @@
       <c r="M5" t="s">
         <v>67</v>
       </c>
-      <c r="N5" t="s">
-        <v>127</v>
-      </c>
-      <c r="O5">
+      <c r="N5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1781,14 +1650,11 @@
       <c r="M6" t="s">
         <v>72</v>
       </c>
-      <c r="N6" t="s">
-        <v>130</v>
-      </c>
-      <c r="O6">
+      <c r="N6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1814,14 +1680,11 @@
       <c r="M7" t="s">
         <v>71</v>
       </c>
-      <c r="N7" t="s">
-        <v>129</v>
-      </c>
-      <c r="O7">
+      <c r="N7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1851,14 +1714,11 @@
       <c r="M8" t="s">
         <v>96</v>
       </c>
-      <c r="N8" t="s">
-        <v>131</v>
-      </c>
-      <c r="O8">
+      <c r="N8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1888,14 +1748,11 @@
       <c r="M9" t="s">
         <v>68</v>
       </c>
-      <c r="N9" t="s">
-        <v>128</v>
-      </c>
-      <c r="O9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1925,14 +1782,11 @@
       <c r="M10" t="s">
         <v>97</v>
       </c>
-      <c r="N10" t="s">
-        <v>132</v>
-      </c>
-      <c r="O10">
+      <c r="N10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1960,16 +1814,13 @@
         <v>62</v>
       </c>
       <c r="M11" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" t="s">
-        <v>133</v>
-      </c>
-      <c r="O11">
+        <v>55</v>
+      </c>
+      <c r="N11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1996,12 +1847,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2018,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -7562,38 +7413,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="K1:M1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"A0005B0036"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"A0025B0034"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"A0019B0032"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"A0019B0029"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"A0017B0029"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"A0018B0042"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"A0019B0031"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"A0009B0029"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"A0008B0029"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"A0008B0030"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"A0005B0036"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>